<commit_message>
add bakwagens and ingroei datasheet
</commit_message>
<xml_diff>
--- a/data_template.xlsx
+++ b/data_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Documents\GitHub\bedrijven_dashboard_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B1EB78-449B-4BAA-B7C4-92E7D41C04BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A12CB24-D428-481D-A702-368E96A33E9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -586,8 +586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -727,10 +727,10 @@
         <v>13</v>
       </c>
       <c r="E2" s="5">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="F2" s="5">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="G2" s="5">
         <v>0</v>
@@ -745,10 +745,10 @@
         <v>15</v>
       </c>
       <c r="K2" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L2" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M2" s="5">
         <v>0</v>
@@ -765,8 +765,8 @@
       <c r="T2" s="13">
         <v>45494</v>
       </c>
-      <c r="U2" s="5">
-        <v>18200</v>
+      <c r="U2" s="13">
+        <v>45494</v>
       </c>
       <c r="V2" s="5">
         <v>18000</v>

</xml_diff>

<commit_message>
add sbi code 4941
</commit_message>
<xml_diff>
--- a/data_template.xlsx
+++ b/data_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Documents\GitHub\bedrijven_dashboard_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59D5D536-9174-462F-871F-3BD8CB0EFC01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E4A2A05-7885-4667-AF90-E1BF28EF058E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,20 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$S$1:$S$163</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -61,9 +74,6 @@
     <t>Groothandel zonder koeling</t>
   </si>
   <si>
-    <t>LOGISTIEK</t>
-  </si>
-  <si>
     <t>fossiel trucks</t>
   </si>
   <si>
@@ -122,6 +132,9 @@
   </si>
   <si>
     <t>smart</t>
+  </si>
+  <si>
+    <t>SBI_4941</t>
   </si>
 </sst>
 </file>
@@ -567,8 +580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC163"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -605,13 +618,13 @@
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>1</v>
@@ -626,16 +639,16 @@
         <v>4</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="L1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="N1" s="7" t="s">
         <v>6</v>
@@ -647,43 +660,43 @@
         <v>8</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="T1" s="4" t="s">
         <v>10</v>
       </c>
       <c r="U1" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="V1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="9" t="s">
+      <c r="W1" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="X1" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y1" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="11" t="s">
+      <c r="AA1" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB1" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="X1" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y1" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z1" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA1" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="AB1" s="11" t="s">
+      <c r="AC1" s="10" t="s">
         <v>26</v>
-      </c>
-      <c r="AC1" s="10" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:29">
@@ -691,7 +704,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" s="5">
         <v>23</v>
@@ -709,7 +722,7 @@
         <v>11</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="I2" s="5">
         <v>2</v>
@@ -721,10 +734,10 @@
         <v>0</v>
       </c>
       <c r="L2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="M2" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>32</v>
       </c>
       <c r="Q2" s="5">
         <v>900000</v>

</xml_diff>

<commit_message>
change back to LOGISTIEK
</commit_message>
<xml_diff>
--- a/data_template.xlsx
+++ b/data_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Documents\GitHub\bedrijven_dashboard_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E4A2A05-7885-4667-AF90-E1BF28EF058E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{170D02B5-3665-4EC5-960F-698CCCA5F35A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -134,7 +134,7 @@
     <t>smart</t>
   </si>
   <si>
-    <t>SBI_4941</t>
+    <t>LOGISTIEK</t>
   </si>
 </sst>
 </file>
@@ -581,7 +581,7 @@
   <dimension ref="A1:AC163"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>

</xml_diff>